<commit_message>
Divided inventory notebook into background and foreground. Foreground matches to the asphalt database sucessfully. Foreground file must update extra fuel consumption values.
</commit_message>
<xml_diff>
--- a/Foreground.xlsx
+++ b/Foreground.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreavargasf/STI/SustainableTransportationInfra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDE44EA2-E7A8-8E45-9302-AA585701B31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B7CD10-54D0-A244-8C26-847B8CC2238C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="157">
   <si>
     <t>database</t>
   </si>
@@ -234,12 +234,6 @@
   </si>
   <si>
     <t>lime, hydrated, packed</t>
-  </si>
-  <si>
-    <t>B, transport, freight, lorry 7.5-16 metric ton, EURO5</t>
-  </si>
-  <si>
-    <t>B, transport, passenger car, medium size, petrol, EURO 5</t>
   </si>
   <si>
     <t>weak filler</t>
@@ -909,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80E2C30-7F43-7943-BA1E-3403AEEE09C6}">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
-      <selection activeCell="D354" sqref="D354"/>
+    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
+      <selection activeCell="F326" sqref="F326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -940,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -948,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -956,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1136,7 +1130,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1259,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1448,7 +1442,7 @@
         <v>64</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J38" s="1">
         <v>2</v>
@@ -1465,7 +1459,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -1473,7 +1467,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -1654,7 +1648,7 @@
         <v>64</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J51" s="1">
         <v>2</v>
@@ -1693,7 +1687,7 @@
         <v>64</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J52" s="1">
         <v>2</v>
@@ -1711,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -1719,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -1727,7 +1721,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -1900,7 +1894,7 @@
         <v>64</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J65" s="1">
         <v>2</v>
@@ -1939,7 +1933,7 @@
         <v>64</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J66" s="1">
         <v>2</v>
@@ -1957,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -1965,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
@@ -1973,7 +1967,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -2146,7 +2140,7 @@
         <v>64</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J79" s="1">
         <v>2</v>
@@ -2185,7 +2179,7 @@
         <v>64</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J80" s="1">
         <v>2</v>
@@ -2203,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
@@ -2211,7 +2205,7 @@
         <v>2</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -2219,7 +2213,7 @@
         <v>3</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
@@ -2331,10 +2325,10 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>51</v>
@@ -2392,7 +2386,7 @@
         <v>64</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J93" s="1">
         <v>2</v>
@@ -2431,7 +2425,7 @@
         <v>64</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J94" s="1">
         <v>2</v>
@@ -2449,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
@@ -2457,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
@@ -2465,7 +2459,7 @@
         <v>3</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
@@ -2577,10 +2571,10 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>17</v>
@@ -2638,7 +2632,7 @@
         <v>64</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J107" s="1">
         <v>2</v>
@@ -2655,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
@@ -2671,7 +2665,7 @@
         <v>3</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
@@ -2783,7 +2777,7 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>54</v>
@@ -2844,7 +2838,7 @@
         <v>64</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J120" s="1">
         <v>2</v>
@@ -2861,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.2">
@@ -2869,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
@@ -2877,7 +2871,7 @@
         <v>3</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
@@ -3025,7 +3019,7 @@
         <v>64</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J132" s="1">
         <v>2</v>
@@ -3068,7 +3062,7 @@
         <v>64</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J133" s="1">
         <v>2</v>
@@ -3111,7 +3105,7 @@
         <v>64</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J134" s="1">
         <v>2</v>
@@ -3154,7 +3148,7 @@
         <v>64</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J135" s="1">
         <v>2</v>
@@ -3197,7 +3191,7 @@
         <v>64</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J136" s="1">
         <v>2</v>
@@ -3212,10 +3206,10 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>17</v>
@@ -3237,7 +3231,7 @@
         <v>64</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J137" s="1">
         <v>2</v>
@@ -3255,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
@@ -3263,7 +3257,7 @@
         <v>2</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
@@ -3271,7 +3265,7 @@
         <v>3</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
@@ -3419,7 +3413,7 @@
         <v>64</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J149" s="1">
         <v>2</v>
@@ -3462,7 +3456,7 @@
         <v>64</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J150" s="1">
         <v>2</v>
@@ -3505,7 +3499,7 @@
         <v>64</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J151" s="1">
         <v>2</v>
@@ -3548,7 +3542,7 @@
         <v>64</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J152" s="1">
         <v>2</v>
@@ -3591,7 +3585,7 @@
         <v>64</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J153" s="1">
         <v>2</v>
@@ -3634,7 +3628,7 @@
         <v>64</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J154" s="1">
         <v>2</v>
@@ -3652,7 +3646,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.2">
@@ -3660,7 +3654,7 @@
         <v>2</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.2">
@@ -3668,7 +3662,7 @@
         <v>3</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.2">
@@ -3816,7 +3810,7 @@
         <v>64</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J166" s="1">
         <v>2</v>
@@ -3859,7 +3853,7 @@
         <v>64</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J167" s="1">
         <v>2</v>
@@ -3902,7 +3896,7 @@
         <v>64</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J168" s="1">
         <v>2</v>
@@ -3945,7 +3939,7 @@
         <v>64</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J169" s="1">
         <v>2</v>
@@ -3988,7 +3982,7 @@
         <v>64</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J170" s="1">
         <v>2</v>
@@ -4031,7 +4025,7 @@
         <v>64</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J171" s="1">
         <v>2</v>
@@ -4074,7 +4068,7 @@
         <v>64</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J172" s="1">
         <v>2</v>
@@ -4092,7 +4086,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.2">
@@ -4100,7 +4094,7 @@
         <v>2</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.2">
@@ -4108,7 +4102,7 @@
         <v>3</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.2">
@@ -4244,7 +4238,7 @@
         <v>64</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J184" s="1">
         <v>2</v>
@@ -4284,7 +4278,7 @@
         <v>64</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J185" s="1">
         <v>2</v>
@@ -4324,7 +4318,7 @@
         <v>64</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J186" s="1">
         <v>2</v>
@@ -4435,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.2">
@@ -4443,7 +4437,7 @@
         <v>2</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.2">
@@ -4451,7 +4445,7 @@
         <v>3</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.2">
@@ -4587,7 +4581,7 @@
         <v>64</v>
       </c>
       <c r="I201" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J201" s="1">
         <v>2</v>
@@ -4627,7 +4621,7 @@
         <v>64</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J202" s="1">
         <v>2</v>
@@ -4667,7 +4661,7 @@
         <v>64</v>
       </c>
       <c r="I203" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J203" s="1">
         <v>2</v>
@@ -4778,7 +4772,7 @@
         <v>1</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -4786,7 +4780,7 @@
         <v>2</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -4794,7 +4788,7 @@
         <v>3</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -4930,7 +4924,7 @@
         <v>64</v>
       </c>
       <c r="I218" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J218" s="1">
         <v>2</v>
@@ -4970,7 +4964,7 @@
         <v>64</v>
       </c>
       <c r="I219" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J219" s="1">
         <v>2</v>
@@ -5010,7 +5004,7 @@
         <v>64</v>
       </c>
       <c r="I220" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J220" s="1">
         <v>2</v>
@@ -5118,7 +5112,7 @@
         <v>1</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
@@ -5126,7 +5120,7 @@
         <v>2</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -5134,7 +5128,7 @@
         <v>3</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
@@ -5270,7 +5264,7 @@
         <v>64</v>
       </c>
       <c r="I235" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J235" s="1">
         <v>2</v>
@@ -5310,7 +5304,7 @@
         <v>64</v>
       </c>
       <c r="I236" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J236" s="1">
         <v>2</v>
@@ -5328,7 +5322,7 @@
         <v>1</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
@@ -5336,7 +5330,7 @@
         <v>2</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.2">
@@ -5344,7 +5338,7 @@
         <v>3</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.2">
@@ -5498,7 +5492,7 @@
         <v>1</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.2">
@@ -5506,7 +5500,7 @@
         <v>2</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.2">
@@ -5514,7 +5508,7 @@
         <v>3</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.2">
@@ -5626,7 +5620,7 @@
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>63</v>
@@ -5650,7 +5644,7 @@
         <v>64</v>
       </c>
       <c r="I260" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J260" s="1">
         <v>1</v>
@@ -5661,7 +5655,7 @@
         <v>1</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.2">
@@ -5669,7 +5663,7 @@
         <v>2</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.2">
@@ -5677,7 +5671,7 @@
         <v>3</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.2">
@@ -5789,7 +5783,7 @@
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>62</v>
@@ -5813,7 +5807,7 @@
         <v>64</v>
       </c>
       <c r="I272" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J272" s="1">
         <v>1</v>
@@ -5824,7 +5818,7 @@
         <v>1</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.2">
@@ -5832,7 +5826,7 @@
         <v>2</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.2">
@@ -5840,7 +5834,7 @@
         <v>3</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.2">
@@ -5952,7 +5946,7 @@
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>62</v>
@@ -5976,7 +5970,7 @@
         <v>64</v>
       </c>
       <c r="I284" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J284" s="1">
         <v>1</v>
@@ -5987,7 +5981,7 @@
         <v>1</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.2">
@@ -6003,7 +5997,7 @@
         <v>3</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.2">
@@ -6139,7 +6133,7 @@
         <v>64</v>
       </c>
       <c r="I296" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J296" s="1">
         <v>2</v>
@@ -6157,7 +6151,7 @@
         <v>1</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.2">
@@ -6165,7 +6159,7 @@
         <v>2</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.2">
@@ -6173,7 +6167,7 @@
         <v>3</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.2">
@@ -6309,7 +6303,7 @@
         <v>64</v>
       </c>
       <c r="I308" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J308" s="1">
         <v>2</v>
@@ -6349,7 +6343,7 @@
         <v>64</v>
       </c>
       <c r="I309" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J309" s="1">
         <v>2</v>
@@ -6367,7 +6361,7 @@
         <v>1</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.2">
@@ -6383,7 +6377,7 @@
         <v>3</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.2">
@@ -6480,7 +6474,7 @@
         <v>11</v>
       </c>
       <c r="F320" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G320" s="1" t="s">
         <v>20</v>
@@ -6540,7 +6534,7 @@
         <v>1</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.2">
@@ -6556,7 +6550,7 @@
         <v>3</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.2">
@@ -6993,7 +6987,7 @@
         <v>1</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F344" s="2"/>
     </row>
@@ -7011,7 +7005,7 @@
         <v>3</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F346" s="2"/>
     </row>
@@ -7449,7 +7443,7 @@
         <v>1</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F365" s="2"/>
     </row>
@@ -7467,7 +7461,7 @@
         <v>3</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F367" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added pavement structure in the foreground file and static calculations notebook
</commit_message>
<xml_diff>
--- a/Foreground.xlsx
+++ b/Foreground.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreavargasf/STI/SustainableTransportationInfra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B7CD10-54D0-A244-8C26-847B8CC2238C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F951076F-2A84-674C-BEFF-721393980FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="162">
   <si>
     <t>database</t>
   </si>
@@ -504,6 +504,21 @@
   </si>
   <si>
     <t>asphalt_SMA</t>
+  </si>
+  <si>
+    <t>pavement structure</t>
+  </si>
+  <si>
+    <t>pavement_structure</t>
+  </si>
+  <si>
+    <t>AC_surf: density 2350 kg/m3</t>
+  </si>
+  <si>
+    <t>AC_bin: density 2370 kg/m3</t>
+  </si>
+  <si>
+    <t>AC_base: density 2370 kg/m3</t>
   </si>
 </sst>
 </file>
@@ -901,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80E2C30-7F43-7943-BA1E-3403AEEE09C6}">
-  <dimension ref="A1:L384"/>
+  <dimension ref="A1:L405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
-      <selection activeCell="F326" sqref="F326"/>
+    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="E401" sqref="E401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -916,7 +931,7 @@
     <col min="6" max="6" width="18.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.1640625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
@@ -5629,7 +5644,7 @@
         <v>16</v>
       </c>
       <c r="D260" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E260" s="1" t="s">
         <v>65</v>
@@ -5792,7 +5807,7 @@
         <v>16</v>
       </c>
       <c r="D272" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E272" s="1" t="s">
         <v>18</v>
@@ -5955,7 +5970,7 @@
         <v>16</v>
       </c>
       <c r="D284" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E284" s="1" t="s">
         <v>18</v>
@@ -6801,7 +6816,7 @@
         <v>NL</v>
       </c>
       <c r="D337" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E337" s="1" t="s">
         <v>65</v>
@@ -6833,7 +6848,7 @@
         <v>NL</v>
       </c>
       <c r="D338" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E338" s="1" t="s">
         <v>65</v>
@@ -6865,7 +6880,7 @@
         <v>NL</v>
       </c>
       <c r="D339" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E339" s="1" t="s">
         <v>65</v>
@@ -6929,7 +6944,7 @@
         <v>NL</v>
       </c>
       <c r="D341" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E341" s="1" t="s">
         <v>11</v>
@@ -6961,7 +6976,7 @@
         <v>NL</v>
       </c>
       <c r="D342" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E342" s="1" t="s">
         <v>11</v>
@@ -7257,7 +7272,7 @@
         <v>NL</v>
       </c>
       <c r="D358" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E358" s="1" t="s">
         <v>65</v>
@@ -7289,7 +7304,7 @@
         <v>NL</v>
       </c>
       <c r="D359" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E359" s="1" t="s">
         <v>65</v>
@@ -7321,7 +7336,7 @@
         <v>NL</v>
       </c>
       <c r="D360" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E360" s="1" t="s">
         <v>65</v>
@@ -7385,7 +7400,7 @@
         <v>NL</v>
       </c>
       <c r="D362" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E362" s="1" t="s">
         <v>11</v>
@@ -7417,7 +7432,7 @@
         <v>NL</v>
       </c>
       <c r="D363" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E363" s="1" t="s">
         <v>11</v>
@@ -7713,7 +7728,7 @@
         <v>NL</v>
       </c>
       <c r="D379" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>65</v>
@@ -7745,7 +7760,7 @@
         <v>NL</v>
       </c>
       <c r="D380" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E380" s="1" t="s">
         <v>65</v>
@@ -7777,7 +7792,7 @@
         <v>NL</v>
       </c>
       <c r="D381" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E381" s="1" t="s">
         <v>65</v>
@@ -7841,7 +7856,7 @@
         <v>NL</v>
       </c>
       <c r="D383" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E383" s="1" t="s">
         <v>11</v>
@@ -7873,7 +7888,7 @@
         <v>NL</v>
       </c>
       <c r="D384" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E384" s="1" t="s">
         <v>11</v>
@@ -7890,6 +7905,269 @@
       <c r="J384" s="1">
         <v>0</v>
       </c>
+    </row>
+    <row r="386" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F386" s="2"/>
+    </row>
+    <row r="387" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F387" s="2"/>
+    </row>
+    <row r="388" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F388" s="2"/>
+    </row>
+    <row r="389" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="390" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A390" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B390" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="392" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B392" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A393" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="394" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A394" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E394" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I394" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J394" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K394" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L394" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="395" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A395" s="1" t="str">
+        <f>B386</f>
+        <v>pavement structure</v>
+      </c>
+      <c r="B395" s="1" t="str">
+        <f>B387</f>
+        <v>pavement structure</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D395" s="1">
+        <v>1</v>
+      </c>
+      <c r="E395" s="1" t="str">
+        <f>B391</f>
+        <v>kilometer</v>
+      </c>
+      <c r="F395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G395" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H395" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J395" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A396" s="1" t="str">
+        <f>A332</f>
+        <v>AC Surf</v>
+      </c>
+      <c r="B396" s="1" t="str">
+        <f t="shared" ref="B396:C396" si="65">B332</f>
+        <v>asphalt</v>
+      </c>
+      <c r="C396" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NL</v>
+      </c>
+      <c r="D396" s="1">
+        <f>(3.75*6*0.038*1000)*2350</f>
+        <v>2009250</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H396" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I396" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J396" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A397" s="1" t="str">
+        <f>A353</f>
+        <v>AC Bin</v>
+      </c>
+      <c r="B397" s="1" t="str">
+        <f t="shared" ref="B397:C397" si="66">B353</f>
+        <v>asphalt</v>
+      </c>
+      <c r="C397" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NL</v>
+      </c>
+      <c r="D397" s="1">
+        <f>(3.75*6*0.051*1000)*2370</f>
+        <v>2719575</v>
+      </c>
+      <c r="E397" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G397" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H397" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I397" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J397" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A398" s="1" t="str">
+        <f>A353</f>
+        <v>AC Bin</v>
+      </c>
+      <c r="B398" s="1" t="str">
+        <f t="shared" ref="B398:C398" si="67">B353</f>
+        <v>asphalt</v>
+      </c>
+      <c r="C398" s="1" t="str">
+        <f t="shared" si="67"/>
+        <v>NL</v>
+      </c>
+      <c r="D398" s="1">
+        <f>(3.75*6*0.254*1000)*2370</f>
+        <v>13544550</v>
+      </c>
+      <c r="E398" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F398" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G398" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H398" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I398" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J398" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F399" s="2"/>
+    </row>
+    <row r="400" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F400" s="2"/>
+    </row>
+    <row r="401" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F401" s="2"/>
+    </row>
+    <row r="402" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F402" s="2"/>
+    </row>
+    <row r="403" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F403" s="2"/>
+    </row>
+    <row r="404" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F404" s="2"/>
+    </row>
+    <row r="405" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F405" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added stochastic calculations, graphs and GSA
</commit_message>
<xml_diff>
--- a/Foreground.xlsx
+++ b/Foreground.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreavargasf/STI/SustainableTransportationInfra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F951076F-2A84-674C-BEFF-721393980FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0E4428-F1EB-C347-A965-62048FA345BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80E2C30-7F43-7943-BA1E-3403AEEE09C6}">
   <dimension ref="A1:L405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="E401" sqref="E401"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="K321" sqref="K321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1463,7 +1463,8 @@
         <v>2</v>
       </c>
       <c r="K38" s="1">
-        <v>-4.5756113837465469</v>
+        <f>LN(D38)</f>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="L38" s="1">
         <v>0.34745503306183378</v>
@@ -1669,7 +1670,8 @@
         <v>2</v>
       </c>
       <c r="K51" s="1">
-        <v>-4.5756113837465469</v>
+        <f>LN(D51)</f>
+        <v>-3.6888794541139363</v>
       </c>
       <c r="L51" s="1">
         <v>0.34745503306183378</v>
@@ -1708,7 +1710,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="1">
-        <f t="shared" ref="K52" si="2">LN(D52)</f>
+        <f>LN(D52)</f>
         <v>-0.41551544396166579</v>
       </c>
       <c r="L52" s="1">
@@ -1875,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="K64" s="1">
-        <f t="shared" ref="K64" si="3">LN(D64)</f>
+        <f t="shared" ref="K64" si="2">LN(D64)</f>
         <v>0</v>
       </c>
       <c r="L64" s="1">
@@ -1915,7 +1917,8 @@
         <v>2</v>
       </c>
       <c r="K65" s="1">
-        <v>-4.5756113837465469</v>
+        <f>LN(D65)</f>
+        <v>-3.6888794541139363</v>
       </c>
       <c r="L65" s="1">
         <v>0.34745503306183378</v>
@@ -1954,7 +1957,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="1">
-        <f t="shared" ref="K66" si="4">LN(D66)</f>
+        <f>LN(D66)</f>
         <v>-0.41551544396166579</v>
       </c>
       <c r="L66" s="1">
@@ -2121,7 +2124,7 @@
         <v>2</v>
       </c>
       <c r="K78" s="1">
-        <f t="shared" ref="K78" si="5">LN(D78)</f>
+        <f t="shared" ref="K78" si="3">LN(D78)</f>
         <v>0</v>
       </c>
       <c r="L78" s="1">
@@ -2161,7 +2164,8 @@
         <v>2</v>
       </c>
       <c r="K79" s="1">
-        <v>-4.5756113837465469</v>
+        <f>LN(D79)</f>
+        <v>-3.6888794541139363</v>
       </c>
       <c r="L79" s="1">
         <v>0.34745503306183378</v>
@@ -2200,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="K80" s="1">
-        <f t="shared" ref="K80" si="6">LN(D80)</f>
+        <f>LN(D80)</f>
         <v>-1.8971199848858813</v>
       </c>
       <c r="L80" s="1">
@@ -2364,14 +2368,14 @@
         <v>64</v>
       </c>
       <c r="J92" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K92" s="1">
-        <f t="shared" ref="K92" si="7">LN(D92)</f>
+        <f t="shared" ref="K92" si="4">LN(D92)</f>
         <v>0</v>
       </c>
       <c r="L92" s="1">
-        <v>3.7416573867739403E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
@@ -2407,7 +2411,8 @@
         <v>2</v>
       </c>
       <c r="K93" s="1">
-        <v>-4.5756113837465469</v>
+        <f>LN(D93)</f>
+        <v>-3.6888794541139363</v>
       </c>
       <c r="L93" s="1">
         <v>0.34745503306183378</v>
@@ -2446,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="1">
-        <f t="shared" ref="K94" si="8">LN(D94)</f>
+        <f>LN(D94)</f>
         <v>-1.8971199848858813</v>
       </c>
       <c r="L94" s="1">
@@ -2610,14 +2615,14 @@
         <v>64</v>
       </c>
       <c r="J106" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K106" s="1">
-        <f t="shared" ref="K106" si="9">LN(D106)</f>
+        <f t="shared" ref="K106" si="5">LN(D106)</f>
         <v>0</v>
       </c>
       <c r="L106" s="1">
-        <v>3.741657386773941E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
@@ -2653,7 +2658,8 @@
         <v>2</v>
       </c>
       <c r="K107" s="1">
-        <v>-4.5756113837465469</v>
+        <f>LN(D107)</f>
+        <v>-1.9951003932460849</v>
       </c>
       <c r="L107" s="1">
         <v>0.34745503306183378</v>
@@ -2816,14 +2822,14 @@
         <v>64</v>
       </c>
       <c r="J119" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K119" s="1">
-        <f t="shared" ref="K119" si="10">LN(D119)</f>
+        <f t="shared" ref="K119" si="6">LN(D119)</f>
         <v>0</v>
       </c>
       <c r="L119" s="1">
-        <v>3.7416573867739403E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.2">
@@ -2859,7 +2865,8 @@
         <v>2</v>
       </c>
       <c r="K120" s="1">
-        <v>-4.5756113837465469</v>
+        <f>LN(D120)</f>
+        <v>-1.731605546408308</v>
       </c>
       <c r="L120" s="1">
         <v>0.34745503306183378</v>
@@ -2994,14 +3001,14 @@
         <v>64</v>
       </c>
       <c r="J131" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K131" s="1">
-        <f t="shared" ref="K131:K137" si="11">LN(D131)</f>
+        <f t="shared" ref="K131:K137" si="7">LN(D131)</f>
         <v>0</v>
       </c>
       <c r="L131" s="1">
-        <v>3.741657386773941E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
@@ -3040,7 +3047,7 @@
         <v>2</v>
       </c>
       <c r="K132" s="1">
-        <f t="shared" si="11"/>
+        <f>LN(D132)</f>
         <v>-3.0791138824930422</v>
       </c>
       <c r="L132" s="1">
@@ -3053,11 +3060,11 @@
         <v>asphalt granulate, free of burden</v>
       </c>
       <c r="B133" s="1" t="str">
-        <f t="shared" ref="B133:C133" si="12">B25</f>
+        <f t="shared" ref="B133:C133" si="8">B25</f>
         <v>asphalt granulate</v>
       </c>
       <c r="C133" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>NL</v>
       </c>
       <c r="D133" s="1">
@@ -3083,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="K133" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="K133:K137" si="9">LN(D133)</f>
         <v>-1.2241755116434554</v>
       </c>
       <c r="L133" s="1">
@@ -3096,11 +3103,11 @@
         <v>crushed stone, production and transport</v>
       </c>
       <c r="B134" s="1" t="str">
-        <f t="shared" ref="B134:C134" si="13">B49</f>
+        <f t="shared" ref="B134:C134" si="10">B49</f>
         <v xml:space="preserve">crushed stone  </v>
       </c>
       <c r="C134" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>NL</v>
       </c>
       <c r="D134" s="1">
@@ -3126,7 +3133,7 @@
         <v>2</v>
       </c>
       <c r="K134" s="1">
-        <f t="shared" ref="K134" si="14">LN(D134)</f>
+        <f t="shared" si="9"/>
         <v>-1.0051219455807707</v>
       </c>
       <c r="L134" s="1">
@@ -3139,11 +3146,11 @@
         <v>crushed sand, production and transport</v>
       </c>
       <c r="B135" s="1" t="str">
-        <f t="shared" ref="B135:C135" si="15">B63</f>
+        <f t="shared" ref="B135:C135" si="11">B63</f>
         <v xml:space="preserve">crushed sand  </v>
       </c>
       <c r="C135" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>NL</v>
       </c>
       <c r="D135" s="1">
@@ -3169,7 +3176,7 @@
         <v>2</v>
       </c>
       <c r="K135" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-1.3547956940605197</v>
       </c>
       <c r="L135" s="1">
@@ -3182,11 +3189,11 @@
         <v>other fillers, production and transport</v>
       </c>
       <c r="B136" s="1" t="str">
-        <f t="shared" ref="B136:C136" si="16">B77</f>
+        <f t="shared" ref="B136:C136" si="12">B77</f>
         <v>other fillers</v>
       </c>
       <c r="C136" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>NL</v>
       </c>
       <c r="D136" s="1">
@@ -3212,7 +3219,7 @@
         <v>2</v>
       </c>
       <c r="K136" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-4.7105307016459177</v>
       </c>
       <c r="L136" s="1">
@@ -3252,7 +3259,7 @@
         <v>2</v>
       </c>
       <c r="K137" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-3.6119184129778081</v>
       </c>
       <c r="L137" s="1">
@@ -3391,7 +3398,7 @@
         <v>2</v>
       </c>
       <c r="K148" s="1">
-        <f t="shared" ref="K148:K154" si="17">LN(D148)</f>
+        <f t="shared" ref="K148:K154" si="13">LN(D148)</f>
         <v>0</v>
       </c>
       <c r="L148" s="1">
@@ -3404,11 +3411,11 @@
         <v>bitumen, production and transport</v>
       </c>
       <c r="B149" s="1" t="str">
-        <f t="shared" ref="B149:C149" si="18">B36</f>
+        <f t="shared" ref="B149:C149" si="14">B36</f>
         <v>bitumen</v>
       </c>
       <c r="C149" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>NL</v>
       </c>
       <c r="D149" s="1">
@@ -3434,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="K149" s="1">
-        <f t="shared" si="17"/>
+        <f>LN(D149)</f>
         <v>-3.912023005428146</v>
       </c>
       <c r="L149" s="1">
@@ -3447,11 +3454,11 @@
         <v>asphalt granulate, free of burden</v>
       </c>
       <c r="B150" s="1" t="str">
-        <f t="shared" ref="B150:C150" si="19">B25</f>
+        <f t="shared" ref="B150:C150" si="15">B25</f>
         <v>asphalt granulate</v>
       </c>
       <c r="C150" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>NL</v>
       </c>
       <c r="D150" s="1">
@@ -3477,7 +3484,7 @@
         <v>2</v>
       </c>
       <c r="K150" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="K150:K154" si="16">LN(D150)</f>
         <v>-0.69114917789727226</v>
       </c>
       <c r="L150" s="1">
@@ -3490,11 +3497,11 @@
         <v>crushed stone, production and transport</v>
       </c>
       <c r="B151" s="1" t="str">
-        <f t="shared" ref="B151:C151" si="20">B49</f>
+        <f t="shared" ref="B151:C151" si="17">B49</f>
         <v xml:space="preserve">crushed stone  </v>
       </c>
       <c r="C151" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NL</v>
       </c>
       <c r="D151" s="1">
@@ -3520,7 +3527,7 @@
         <v>2</v>
       </c>
       <c r="K151" s="1">
-        <f t="shared" ref="K151" si="21">LN(D151)</f>
+        <f t="shared" si="16"/>
         <v>-1.313043899380298</v>
       </c>
       <c r="L151" s="1">
@@ -3533,11 +3540,11 @@
         <v>other fillers, production and transport</v>
       </c>
       <c r="B152" s="1" t="str">
-        <f t="shared" ref="B152:C152" si="22">B77</f>
+        <f t="shared" ref="B152:C152" si="18">B77</f>
         <v>other fillers</v>
       </c>
       <c r="C152" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>NL</v>
       </c>
       <c r="D152" s="1">
@@ -3563,7 +3570,7 @@
         <v>2</v>
       </c>
       <c r="K152" s="1">
-        <f t="shared" ref="K152:K153" si="23">LN(D152)</f>
+        <f t="shared" si="16"/>
         <v>-4.8283137373023015</v>
       </c>
       <c r="L152" s="1">
@@ -3576,11 +3583,11 @@
         <v>natural sand, production and transport</v>
       </c>
       <c r="B153" s="1" t="str">
-        <f t="shared" ref="B153:C153" si="24">B91</f>
+        <f t="shared" ref="B153:C153" si="19">B91</f>
         <v>natural sand</v>
       </c>
       <c r="C153" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>NL</v>
       </c>
       <c r="D153" s="1">
@@ -3606,7 +3613,7 @@
         <v>2</v>
       </c>
       <c r="K153" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="16"/>
         <v>-1.6502599069543555</v>
       </c>
       <c r="L153" s="1">
@@ -3619,11 +3626,11 @@
         <v>weak filler, production and transport</v>
       </c>
       <c r="B154" s="1" t="str">
-        <f t="shared" ref="B154:C154" si="25">B105</f>
+        <f t="shared" ref="B154:C154" si="20">B105</f>
         <v>weak_filler</v>
       </c>
       <c r="C154" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>NL</v>
       </c>
       <c r="D154" s="1">
@@ -3649,7 +3656,7 @@
         <v>2</v>
       </c>
       <c r="K154" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>-4.6051701859880909</v>
       </c>
       <c r="L154" s="1">
@@ -3788,7 +3795,7 @@
         <v>2</v>
       </c>
       <c r="K165" s="1">
-        <f t="shared" ref="K165:K171" si="26">LN(D165)</f>
+        <f t="shared" ref="K165:K171" si="21">LN(D165)</f>
         <v>0</v>
       </c>
       <c r="L165" s="1">
@@ -3801,11 +3808,11 @@
         <v>bitumen, production and transport</v>
       </c>
       <c r="B166" s="1" t="str">
-        <f t="shared" ref="B166:C166" si="27">B36</f>
+        <f t="shared" ref="B166:C166" si="22">B36</f>
         <v>bitumen</v>
       </c>
       <c r="C166" s="1" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>NL</v>
       </c>
       <c r="D166" s="1">
@@ -3831,7 +3838,7 @@
         <v>2</v>
       </c>
       <c r="K166" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>-2.6882475738060303</v>
       </c>
       <c r="L166" s="1">
@@ -3844,11 +3851,11 @@
         <v>crushed stone, production and transport</v>
       </c>
       <c r="B167" s="1" t="str">
-        <f t="shared" ref="B167:C167" si="28">B49</f>
+        <f t="shared" ref="B167:C167" si="23">B49</f>
         <v xml:space="preserve">crushed stone  </v>
       </c>
       <c r="C167" s="1" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>NL</v>
       </c>
       <c r="D167" s="1">
@@ -3874,7 +3881,7 @@
         <v>2</v>
       </c>
       <c r="K167" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>-0.39156220293917288</v>
       </c>
       <c r="L167" s="1">
@@ -3887,11 +3894,11 @@
         <v>crushed sand, production and transport</v>
       </c>
       <c r="B168" s="1" t="str">
-        <f t="shared" ref="B168:C168" si="29">B63</f>
+        <f t="shared" ref="B168:C168" si="24">B63</f>
         <v xml:space="preserve">crushed sand  </v>
       </c>
       <c r="C168" s="1" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>NL</v>
       </c>
       <c r="D168" s="1">
@@ -3917,7 +3924,7 @@
         <v>2</v>
       </c>
       <c r="K168" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>-2.5902671654458267</v>
       </c>
       <c r="L168" s="1">
@@ -3930,11 +3937,11 @@
         <v>other fillers, production and transport</v>
       </c>
       <c r="B169" s="1" t="str">
-        <f t="shared" ref="B169:C169" si="30">B77</f>
+        <f t="shared" ref="B169:C169" si="25">B77</f>
         <v>other fillers</v>
       </c>
       <c r="C169" s="1" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>NL</v>
       </c>
       <c r="D169" s="1">
@@ -3960,7 +3967,7 @@
         <v>2</v>
       </c>
       <c r="K169" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>-2.3968957724652871</v>
       </c>
       <c r="L169" s="1">
@@ -3973,11 +3980,11 @@
         <v>natural sand, production and transport</v>
       </c>
       <c r="B170" s="1" t="str">
-        <f t="shared" ref="B170:C170" si="31">B91</f>
+        <f t="shared" ref="B170:C170" si="26">B91</f>
         <v>natural sand</v>
       </c>
       <c r="C170" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>NL</v>
       </c>
       <c r="D170" s="1">
@@ -4003,7 +4010,7 @@
         <v>2</v>
       </c>
       <c r="K170" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>-2.6172958378337459</v>
       </c>
       <c r="L170" s="1">
@@ -4016,11 +4023,11 @@
         <v>weak filler, production and transport</v>
       </c>
       <c r="B171" s="1" t="str">
-        <f t="shared" ref="B171:C171" si="32">B105</f>
+        <f t="shared" ref="B171:C171" si="27">B105</f>
         <v>weak_filler</v>
       </c>
       <c r="C171" s="1" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>NL</v>
       </c>
       <c r="D171" s="1">
@@ -4046,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="K171" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>-4.2686979493668789</v>
       </c>
       <c r="L171" s="1">
@@ -4059,11 +4066,11 @@
         <v>drip resistant material, production and transport</v>
       </c>
       <c r="B172" s="1" t="str">
-        <f t="shared" ref="B172:C172" si="33">B118</f>
+        <f t="shared" ref="B172:C172" si="28">B118</f>
         <v>drip resistant material</v>
       </c>
       <c r="C172" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>NL</v>
       </c>
       <c r="D172" s="1">
@@ -4089,7 +4096,7 @@
         <v>2</v>
       </c>
       <c r="K172" s="1">
-        <f t="shared" ref="K172" si="34">LN(D172)</f>
+        <f t="shared" ref="K172" si="29">LN(D172)</f>
         <v>-5.8091429903140277</v>
       </c>
       <c r="L172" s="1">
@@ -4259,7 +4266,7 @@
         <v>2</v>
       </c>
       <c r="K184" s="1">
-        <f t="shared" ref="K184:K186" si="35">LN(D184)</f>
+        <f t="shared" ref="K184:K186" si="30">LN(D184)</f>
         <v>-5.1361985170716018</v>
       </c>
       <c r="L184" s="1">
@@ -4299,7 +4306,7 @@
         <v>2</v>
       </c>
       <c r="K185" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>-1.2349011940243562</v>
       </c>
       <c r="L185" s="1">
@@ -4339,7 +4346,7 @@
         <v>2</v>
       </c>
       <c r="K186" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>-5.4500709217755734</v>
       </c>
       <c r="L186" s="1">
@@ -4602,7 +4609,7 @@
         <v>2</v>
       </c>
       <c r="K201" s="1">
-        <f t="shared" ref="K201:K203" si="36">LN(D201)</f>
+        <f t="shared" ref="K201:K203" si="31">LN(D201)</f>
         <v>-5.4284260518950571</v>
       </c>
       <c r="L201" s="1">
@@ -4642,7 +4649,7 @@
         <v>2</v>
       </c>
       <c r="K202" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="31"/>
         <v>-1.2262337508141881</v>
       </c>
       <c r="L202" s="1">
@@ -4682,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="K203" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="31"/>
         <v>-5.4500709217755734</v>
       </c>
       <c r="L203" s="1">
@@ -4945,7 +4952,7 @@
         <v>2</v>
       </c>
       <c r="K218" s="1">
-        <f t="shared" ref="K218:K220" si="37">LN(D218)</f>
+        <f t="shared" ref="K218:K220" si="32">LN(D218)</f>
         <v>-4.9420425026306445</v>
       </c>
       <c r="L218" s="1">
@@ -4985,7 +4992,7 @@
         <v>2</v>
       </c>
       <c r="K219" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>-1.3710787085135288</v>
       </c>
       <c r="L219" s="1">
@@ -5025,7 +5032,7 @@
         <v>2</v>
       </c>
       <c r="K220" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>-5.4500709217755734</v>
       </c>
       <c r="L220" s="1">
@@ -5285,7 +5292,7 @@
         <v>2</v>
       </c>
       <c r="K235" s="1">
-        <f t="shared" ref="K235:K236" si="38">LN(D235)</f>
+        <f t="shared" ref="K235:K236" si="33">LN(D235)</f>
         <v>-3.4021978819957388</v>
       </c>
       <c r="L235" s="1">
@@ -5325,7 +5332,7 @@
         <v>2</v>
       </c>
       <c r="K236" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>-4.5008101706638488</v>
       </c>
       <c r="L236" s="1">
@@ -5495,7 +5502,7 @@
         <v>2</v>
       </c>
       <c r="K248" s="1">
-        <f t="shared" ref="K248" si="39">LN(D248)</f>
+        <f t="shared" ref="K248" si="34">LN(D248)</f>
         <v>-4.4688925676955433</v>
       </c>
       <c r="L248" s="1">
@@ -5662,7 +5669,7 @@
         <v>147</v>
       </c>
       <c r="J260" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.2">
@@ -5825,7 +5832,7 @@
         <v>148</v>
       </c>
       <c r="J272" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.2">
@@ -5988,7 +5995,7 @@
         <v>149</v>
       </c>
       <c r="J284" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.2">
@@ -6154,7 +6161,7 @@
         <v>2</v>
       </c>
       <c r="K296" s="1">
-        <f t="shared" ref="K296" si="40">LN(D296)</f>
+        <f t="shared" ref="K296" si="35">LN(D296)</f>
         <v>-3.5913172665291841</v>
       </c>
       <c r="L296" s="1">
@@ -6324,7 +6331,7 @@
         <v>2</v>
       </c>
       <c r="K308" s="1">
-        <f t="shared" ref="K308:K309" si="41">LN(D308)</f>
+        <f t="shared" ref="K308:K309" si="36">LN(D308)</f>
         <v>-3.4021978819957388</v>
       </c>
       <c r="L308" s="1">
@@ -6364,7 +6371,7 @@
         <v>2</v>
       </c>
       <c r="K309" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="36"/>
         <v>-4.5008101706638488</v>
       </c>
       <c r="L309" s="1">
@@ -6534,7 +6541,7 @@
         <v>2</v>
       </c>
       <c r="K321" s="1">
-        <f t="shared" ref="K321" si="42">LN(D321)</f>
+        <f t="shared" ref="K321" si="37">LN(D321)</f>
         <v>-4.3240596589193494</v>
       </c>
       <c r="L321" s="1">
@@ -6680,11 +6687,11 @@
         <v>AC Surf, materials and transport to plant</v>
       </c>
       <c r="B333" s="1" t="str">
-        <f t="shared" ref="B333:C333" si="43">B131</f>
+        <f t="shared" ref="B333:C333" si="38">B131</f>
         <v>AC Surf</v>
       </c>
       <c r="C333" s="1" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>NL</v>
       </c>
       <c r="D333" s="1">
@@ -6712,11 +6719,11 @@
         <v>AC Surf, production</v>
       </c>
       <c r="B334" s="1" t="str">
-        <f t="shared" ref="B334:C334" si="44">B183</f>
+        <f t="shared" ref="B334:C334" si="39">B183</f>
         <v xml:space="preserve">AC Surf </v>
       </c>
       <c r="C334" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>NL</v>
       </c>
       <c r="D334" s="1">
@@ -6744,11 +6751,11 @@
         <v>asphalt, transport to site</v>
       </c>
       <c r="B335" s="1" t="str">
-        <f t="shared" ref="B335:C335" si="45">B234</f>
+        <f t="shared" ref="B335:C335" si="40">B234</f>
         <v>asphalt, transport to site</v>
       </c>
       <c r="C335" s="1" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>NL</v>
       </c>
       <c r="D335" s="1">
@@ -6776,11 +6783,11 @@
         <v>asphalt, construction</v>
       </c>
       <c r="B336" s="1" t="str">
-        <f t="shared" ref="B336:C336" si="46">B247</f>
+        <f t="shared" ref="B336:C336" si="41">B247</f>
         <v xml:space="preserve">asphalt </v>
       </c>
       <c r="C336" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="41"/>
         <v>NL</v>
       </c>
       <c r="D336" s="1">
@@ -6808,11 +6815,11 @@
         <v>asphalt, pvi, car</v>
       </c>
       <c r="B337" s="1" t="str">
-        <f t="shared" ref="B337:C337" si="47">B259</f>
+        <f t="shared" ref="B337:C337" si="42">B259</f>
         <v>extra fuel consumption</v>
       </c>
       <c r="C337" s="1" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="42"/>
         <v>NL</v>
       </c>
       <c r="D337" s="1">
@@ -6840,11 +6847,11 @@
         <v>asphalt, pvi, HDV</v>
       </c>
       <c r="B338" s="1" t="str">
-        <f t="shared" ref="B338:C338" si="48">B271</f>
+        <f t="shared" ref="B338:C338" si="43">B271</f>
         <v>extra fuel consumption</v>
       </c>
       <c r="C338" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="43"/>
         <v>NL</v>
       </c>
       <c r="D338" s="1">
@@ -6872,11 +6879,11 @@
         <v>asphalt, pvi, trailer</v>
       </c>
       <c r="B339" s="1" t="str">
-        <f t="shared" ref="B339:C339" si="49">B283</f>
+        <f t="shared" ref="B339:C339" si="44">B283</f>
         <v>extra fuel consumption</v>
       </c>
       <c r="C339" s="1" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="44"/>
         <v>NL</v>
       </c>
       <c r="D339" s="1">
@@ -6904,11 +6911,11 @@
         <v>asphalt, demolition</v>
       </c>
       <c r="B340" s="1" t="str">
-        <f t="shared" ref="B340:C340" si="50">B295</f>
+        <f t="shared" ref="B340:C340" si="45">B295</f>
         <v>asphalt</v>
       </c>
       <c r="C340" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="45"/>
         <v>NL</v>
       </c>
       <c r="D340" s="1">
@@ -6936,11 +6943,11 @@
         <v>asphalt, transport to processing</v>
       </c>
       <c r="B341" s="1" t="str">
-        <f t="shared" ref="B341:C341" si="51">B307</f>
+        <f t="shared" ref="B341:C341" si="46">B307</f>
         <v xml:space="preserve">asphalt </v>
       </c>
       <c r="C341" s="1" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>NL</v>
       </c>
       <c r="D341" s="1">
@@ -6968,11 +6975,11 @@
         <v>asphalt, processing</v>
       </c>
       <c r="B342" s="1" t="str">
-        <f t="shared" ref="B342:C342" si="52">B320</f>
+        <f t="shared" ref="B342:C342" si="47">B320</f>
         <v>asphalt</v>
       </c>
       <c r="C342" s="1" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>NL</v>
       </c>
       <c r="D342" s="1">
@@ -7136,11 +7143,11 @@
         <v>AC Bin, materials and transport to plant</v>
       </c>
       <c r="B354" s="1" t="str">
-        <f t="shared" ref="B354:C354" si="53">B148</f>
+        <f t="shared" ref="B354:C354" si="48">B148</f>
         <v>AC Bin</v>
       </c>
       <c r="C354" s="1" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="48"/>
         <v>NL</v>
       </c>
       <c r="D354" s="1">
@@ -7168,11 +7175,11 @@
         <v>AC Bin, production</v>
       </c>
       <c r="B355" s="1" t="str">
-        <f t="shared" ref="B355:C355" si="54">B200</f>
+        <f t="shared" ref="B355:C355" si="49">B200</f>
         <v>AC Bin</v>
       </c>
       <c r="C355" s="1" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>NL</v>
       </c>
       <c r="D355" s="1">
@@ -7200,11 +7207,11 @@
         <v>asphalt, transport to site</v>
       </c>
       <c r="B356" s="1" t="str">
-        <f t="shared" ref="B356:C356" si="55">B335</f>
+        <f t="shared" ref="B356:C356" si="50">B335</f>
         <v>asphalt, transport to site</v>
       </c>
       <c r="C356" s="1" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>NL</v>
       </c>
       <c r="D356" s="1">
@@ -7228,15 +7235,15 @@
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="str">
-        <f t="shared" ref="A357:C363" si="56">A336</f>
+        <f t="shared" ref="A357:C363" si="51">A336</f>
         <v>asphalt, construction</v>
       </c>
       <c r="B357" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">asphalt </v>
       </c>
       <c r="C357" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>NL</v>
       </c>
       <c r="D357" s="1">
@@ -7260,15 +7267,15 @@
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt, pvi, car</v>
       </c>
       <c r="B358" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>extra fuel consumption</v>
       </c>
       <c r="C358" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>NL</v>
       </c>
       <c r="D358" s="1">
@@ -7292,15 +7299,15 @@
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt, pvi, HDV</v>
       </c>
       <c r="B359" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>extra fuel consumption</v>
       </c>
       <c r="C359" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>NL</v>
       </c>
       <c r="D359" s="1">
@@ -7324,15 +7331,15 @@
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt, pvi, trailer</v>
       </c>
       <c r="B360" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>extra fuel consumption</v>
       </c>
       <c r="C360" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>NL</v>
       </c>
       <c r="D360" s="1">
@@ -7356,15 +7363,15 @@
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt, demolition</v>
       </c>
       <c r="B361" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt</v>
       </c>
       <c r="C361" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>NL</v>
       </c>
       <c r="D361" s="1">
@@ -7388,15 +7395,15 @@
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt, transport to processing</v>
       </c>
       <c r="B362" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">asphalt </v>
       </c>
       <c r="C362" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>NL</v>
       </c>
       <c r="D362" s="1">
@@ -7420,15 +7427,15 @@
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt, processing</v>
       </c>
       <c r="B363" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>asphalt</v>
       </c>
       <c r="C363" s="1" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>NL</v>
       </c>
       <c r="D363" s="1">
@@ -7656,205 +7663,205 @@
         <v>asphalt, transport to site</v>
       </c>
       <c r="B377" s="1" t="str">
-        <f t="shared" ref="B377:C377" si="57">B356</f>
+        <f t="shared" ref="B377:C377" si="52">B356</f>
         <v>asphalt, transport to site</v>
       </c>
       <c r="C377" s="1" t="str">
+        <f t="shared" si="52"/>
+        <v>NL</v>
+      </c>
+      <c r="D377" s="1">
+        <v>1</v>
+      </c>
+      <c r="E377" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H377" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J377" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A378" s="1" t="str">
+        <f t="shared" ref="A378:C378" si="53">A357</f>
+        <v>asphalt, construction</v>
+      </c>
+      <c r="B378" s="1" t="str">
+        <f t="shared" si="53"/>
+        <v xml:space="preserve">asphalt </v>
+      </c>
+      <c r="C378" s="1" t="str">
+        <f t="shared" si="53"/>
+        <v>NL</v>
+      </c>
+      <c r="D378" s="1">
+        <v>1</v>
+      </c>
+      <c r="E378" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J378" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A379" s="1" t="str">
+        <f t="shared" ref="A379:C379" si="54">A358</f>
+        <v>asphalt, pvi, car</v>
+      </c>
+      <c r="B379" s="1" t="str">
+        <f t="shared" si="54"/>
+        <v>extra fuel consumption</v>
+      </c>
+      <c r="C379" s="1" t="str">
+        <f t="shared" si="54"/>
+        <v>NL</v>
+      </c>
+      <c r="D379" s="1">
+        <v>0</v>
+      </c>
+      <c r="E379" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G379" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H379" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J379" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A380" s="1" t="str">
+        <f t="shared" ref="A380:C380" si="55">A359</f>
+        <v>asphalt, pvi, HDV</v>
+      </c>
+      <c r="B380" s="1" t="str">
+        <f t="shared" si="55"/>
+        <v>extra fuel consumption</v>
+      </c>
+      <c r="C380" s="1" t="str">
+        <f t="shared" si="55"/>
+        <v>NL</v>
+      </c>
+      <c r="D380" s="1">
+        <v>0</v>
+      </c>
+      <c r="E380" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J380" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A381" s="1" t="str">
+        <f t="shared" ref="A381:C381" si="56">A360</f>
+        <v>asphalt, pvi, trailer</v>
+      </c>
+      <c r="B381" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>extra fuel consumption</v>
+      </c>
+      <c r="C381" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>NL</v>
+      </c>
+      <c r="D381" s="1">
+        <v>0</v>
+      </c>
+      <c r="E381" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G381" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H381" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J381" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="str">
+        <f t="shared" ref="A382:C382" si="57">A361</f>
+        <v>asphalt, demolition</v>
+      </c>
+      <c r="B382" s="1" t="str">
+        <f t="shared" si="57"/>
+        <v>asphalt</v>
+      </c>
+      <c r="C382" s="1" t="str">
         <f t="shared" si="57"/>
         <v>NL</v>
       </c>
-      <c r="D377" s="1">
-        <v>1</v>
-      </c>
-      <c r="E377" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F377" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G377" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H377" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J377" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A378" s="1" t="str">
-        <f t="shared" ref="A378:C378" si="58">A357</f>
-        <v>asphalt, construction</v>
-      </c>
-      <c r="B378" s="1" t="str">
+      <c r="D382" s="1">
+        <v>1</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J382" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="str">
+        <f t="shared" ref="A383:C383" si="58">A362</f>
+        <v>asphalt, transport to processing</v>
+      </c>
+      <c r="B383" s="1" t="str">
         <f t="shared" si="58"/>
         <v xml:space="preserve">asphalt </v>
       </c>
-      <c r="C378" s="1" t="str">
+      <c r="C383" s="1" t="str">
         <f t="shared" si="58"/>
         <v>NL</v>
       </c>
-      <c r="D378" s="1">
-        <v>1</v>
-      </c>
-      <c r="E378" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F378" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G378" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H378" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J378" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A379" s="1" t="str">
-        <f t="shared" ref="A379:C379" si="59">A358</f>
-        <v>asphalt, pvi, car</v>
-      </c>
-      <c r="B379" s="1" t="str">
-        <f t="shared" si="59"/>
-        <v>extra fuel consumption</v>
-      </c>
-      <c r="C379" s="1" t="str">
-        <f t="shared" si="59"/>
-        <v>NL</v>
-      </c>
-      <c r="D379" s="1">
-        <v>0</v>
-      </c>
-      <c r="E379" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F379" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G379" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H379" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J379" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A380" s="1" t="str">
-        <f t="shared" ref="A380:C380" si="60">A359</f>
-        <v>asphalt, pvi, HDV</v>
-      </c>
-      <c r="B380" s="1" t="str">
-        <f t="shared" si="60"/>
-        <v>extra fuel consumption</v>
-      </c>
-      <c r="C380" s="1" t="str">
-        <f t="shared" si="60"/>
-        <v>NL</v>
-      </c>
-      <c r="D380" s="1">
-        <v>0</v>
-      </c>
-      <c r="E380" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F380" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G380" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H380" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J380" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A381" s="1" t="str">
-        <f t="shared" ref="A381:C381" si="61">A360</f>
-        <v>asphalt, pvi, trailer</v>
-      </c>
-      <c r="B381" s="1" t="str">
-        <f t="shared" si="61"/>
-        <v>extra fuel consumption</v>
-      </c>
-      <c r="C381" s="1" t="str">
-        <f t="shared" si="61"/>
-        <v>NL</v>
-      </c>
-      <c r="D381" s="1">
-        <v>0</v>
-      </c>
-      <c r="E381" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F381" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G381" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H381" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J381" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A382" s="1" t="str">
-        <f t="shared" ref="A382:C382" si="62">A361</f>
-        <v>asphalt, demolition</v>
-      </c>
-      <c r="B382" s="1" t="str">
-        <f t="shared" si="62"/>
-        <v>asphalt</v>
-      </c>
-      <c r="C382" s="1" t="str">
-        <f t="shared" si="62"/>
-        <v>NL</v>
-      </c>
-      <c r="D382" s="1">
-        <v>1</v>
-      </c>
-      <c r="E382" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F382" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G382" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H382" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J382" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A383" s="1" t="str">
-        <f t="shared" ref="A383:C383" si="63">A362</f>
-        <v>asphalt, transport to processing</v>
-      </c>
-      <c r="B383" s="1" t="str">
-        <f t="shared" si="63"/>
-        <v xml:space="preserve">asphalt </v>
-      </c>
-      <c r="C383" s="1" t="str">
-        <f t="shared" si="63"/>
-        <v>NL</v>
-      </c>
       <c r="D383" s="1">
         <v>0</v>
       </c>
@@ -7876,15 +7883,15 @@
     </row>
     <row r="384" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="str">
-        <f t="shared" ref="A384:C384" si="64">A363</f>
+        <f t="shared" ref="A384:C384" si="59">A363</f>
         <v>asphalt, processing</v>
       </c>
       <c r="B384" s="1" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="59"/>
         <v>asphalt</v>
       </c>
       <c r="C384" s="1" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="59"/>
         <v>NL</v>
       </c>
       <c r="D384" s="1">
@@ -8046,11 +8053,11 @@
         <v>AC Surf</v>
       </c>
       <c r="B396" s="1" t="str">
-        <f t="shared" ref="B396:C396" si="65">B332</f>
+        <f t="shared" ref="B396:C396" si="60">B332</f>
         <v>asphalt</v>
       </c>
       <c r="C396" s="1" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="60"/>
         <v>NL</v>
       </c>
       <c r="D396" s="1">
@@ -8082,11 +8089,11 @@
         <v>AC Bin</v>
       </c>
       <c r="B397" s="1" t="str">
-        <f t="shared" ref="B397:C397" si="66">B353</f>
+        <f t="shared" ref="B397:C397" si="61">B353</f>
         <v>asphalt</v>
       </c>
       <c r="C397" s="1" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="61"/>
         <v>NL</v>
       </c>
       <c r="D397" s="1">
@@ -8118,11 +8125,11 @@
         <v>AC Bin</v>
       </c>
       <c r="B398" s="1" t="str">
-        <f t="shared" ref="B398:C398" si="67">B353</f>
+        <f t="shared" ref="B398:C398" si="62">B353</f>
         <v>asphalt</v>
       </c>
       <c r="C398" s="1" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="62"/>
         <v>NL</v>
       </c>
       <c r="D398" s="1">

</xml_diff>

<commit_message>
Final foreground excel and notebook update
</commit_message>
<xml_diff>
--- a/Foreground.xlsx
+++ b/Foreground.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreavargasf/ua_pmlca/ua_pmlca/scenario uncertainty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2B9775-D1CC-B140-BDF4-279B2F5B461A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A62439-5A78-184D-82EE-6DD5A7A593E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30640" yWindow="500" windowWidth="35280" windowHeight="21660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="2300" yWindow="2320" windowWidth="26840" windowHeight="15860" xr2:uid="{3D4CC386-E372-A94E-B658-9166ADA58240}"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="179">
   <si>
     <t>database</t>
   </si>
@@ -565,6 +565,12 @@
   </si>
   <si>
     <t>pavement structure, AC Surf, 0% RAP, modified bitumen</t>
+  </si>
+  <si>
+    <t>pavement_structure_4</t>
+  </si>
+  <si>
+    <t>asphalt_AC_Surf_4</t>
   </si>
 </sst>
 </file>
@@ -965,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80E2C30-7F43-7943-BA1E-3403AEEE09C6}">
   <dimension ref="A1:L546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A501" workbookViewId="0">
-      <selection activeCell="B534" sqref="B534"/>
+    <sheetView tabSelected="1" topLeftCell="A389" workbookViewId="0">
+      <selection activeCell="B440" sqref="B440"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="A419" workbookViewId="1"/>
   </sheetViews>
@@ -9124,7 +9130,7 @@
         <v>3</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="441" spans="1:12" x14ac:dyDescent="0.2">
@@ -10771,15 +10777,16 @@
     </row>
     <row r="529" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A529" s="1" t="str">
-        <f>A429</f>
-        <v>AC Surf, 0% RAP, regular bitumen</v>
+        <f>B520</f>
+        <v>pavement structure, AC Surf, 0% RAP, regular bitumen</v>
       </c>
       <c r="B529" s="1" t="str">
         <f>B521</f>
         <v>pavement structure</v>
       </c>
-      <c r="C529" s="1" t="s">
-        <v>17</v>
+      <c r="C529" s="1" t="str">
+        <f>B523</f>
+        <v>NL</v>
       </c>
       <c r="D529" s="1">
         <v>1</v>
@@ -10935,7 +10942,7 @@
         <v>3</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F536" s="2"/>
     </row>

</xml_diff>